<commit_message>
The mag field is not pointing in the right direction
</commit_message>
<xml_diff>
--- a/MAIN/0 - MAIN/currentdata.xlsx
+++ b/MAIN/0 - MAIN/currentdata.xlsx
@@ -401,7 +401,7 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -412,7 +412,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -423,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -445,7 +445,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -456,7 +456,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -478,1107 +478,1107 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>-716.44896031344524</v>
+        <v>-3535533905.9327378</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>-36.786078963253956</v>
+        <v>-213014277.34684983</v>
       </c>
       <c r="B9">
-        <v>130.53953954319013</v>
+        <v>755905126.73991954</v>
       </c>
       <c r="C9">
-        <v>-638.01278921192647</v>
+        <v>-3694490879.7641759</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>-54.099206202966997</v>
+        <v>-367444310.4161849</v>
       </c>
       <c r="B10">
-        <v>231.66766242614287</v>
+        <v>1573497476.9599299</v>
       </c>
       <c r="C10">
-        <v>-525.87444037510852</v>
+        <v>-3571763518.7506952</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>-56.447336332563559</v>
+        <v>-449350340.0023278</v>
       </c>
       <c r="B11">
-        <v>300.17837780764262</v>
+        <v>2389576991.4549232</v>
       </c>
       <c r="C11">
-        <v>-393.00612027258762</v>
+        <v>-3128534404.6536837</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <v>-48.729511945579645</v>
+        <v>-454162131.2321834</v>
       </c>
       <c r="B12">
-        <v>336.05145068566611</v>
+        <v>3132020760.1815262</v>
       </c>
       <c r="C12">
-        <v>-251.82497272964537</v>
+        <v>-2347024662.1822958</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <v>-35.584307329539349</v>
+        <v>-387778362.95088977</v>
       </c>
       <c r="B13">
-        <v>341.84924457029342</v>
+        <v>3725286520.483263</v>
       </c>
       <c r="C13">
-        <v>-113.41338008488694</v>
+        <v>-1235917126.5794544</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <v>-20.947581623670136</v>
+        <v>-266505425.51491234</v>
       </c>
       <c r="B14">
-        <v>322.02027651294225</v>
+        <v>4096900174.841053</v>
       </c>
       <c r="C14">
-        <v>13.028961370348151</v>
+        <v>165760848.02545452</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
-        <v>-7.8052231334617987</v>
+        <v>-115737508.85591002</v>
       </c>
       <c r="B15">
-        <v>282.19351968483278</v>
+        <v>4184425534.689116</v>
       </c>
       <c r="C15">
-        <v>120.50977156198904</v>
+        <v>1786944526.1065016</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <v>1.8889497232845789</v>
+        <v>32586552.18478816</v>
       </c>
       <c r="B16">
-        <v>228.52494767876325</v>
+        <v>3942317808.2850971</v>
       </c>
       <c r="C16">
-        <v>204.36681547536304</v>
+        <v>3525562282.1696396</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <v>7.1673075042498366</v>
+        <v>143572482.68287215</v>
       </c>
       <c r="B17">
-        <v>167.13679264112125</v>
+        <v>3348013776.8485117</v>
       </c>
       <c r="C17">
-        <v>262.21768406063535</v>
+        <v>5252634114.2214947</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <v>7.9131238444566039</v>
+        <v>183693677.50607803</v>
       </c>
       <c r="B18">
-        <v>103.67193897484299</v>
+        <v>2406619698.9720383</v>
       </c>
       <c r="C18">
-        <v>293.77056294741988</v>
+        <v>6819531213.1561937</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>4.6718809524710858</v>
+        <v>125423225.20592038</v>
       </c>
       <c r="B19">
-        <v>42.971354346414785</v>
+        <v>1153626538.9517422</v>
       </c>
       <c r="C19">
-        <v>300.53154023136739</v>
+        <v>8068192540.7332392</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <v>-1.5598032261076586</v>
+        <v>-48326732.667755939</v>
       </c>
       <c r="B20">
-        <v>-11.128526497171819</v>
+        <v>-344790494.0912984</v>
       </c>
       <c r="C20">
-        <v>285.44347526794394</v>
+        <v>8843776118.7686005</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>-9.5427447000458212</v>
+        <v>-340488822.96501452</v>
       </c>
       <c r="B21">
-        <v>-55.889307194877986</v>
+        <v>-1994152104.1658747</v>
       </c>
       <c r="C21">
-        <v>252.48920913637656</v>
+        <v>9008912669.5173397</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>-17.982845176103375</v>
+        <v>-737352007.07359278</v>
       </c>
       <c r="B22">
-        <v>-89.670844453670739</v>
+        <v>-3676780647.6897612</v>
       </c>
       <c r="C22">
-        <v>206.288399053006</v>
+        <v>8458459358.8038483</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <v>-25.685608197135132</v>
+        <v>-1207722580.1273038</v>
       </c>
       <c r="B23">
-        <v>-111.85668085849176</v>
+        <v>-5259437042.4898748</v>
       </c>
       <c r="C23">
-        <v>151.71289388608292</v>
+        <v>7133453342.2929173</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <v>-31.670857037326602</v>
+        <v>-1704020253.150903</v>
       </c>
       <c r="B24">
-        <v>-122.72408051572155</v>
+        <v>-6603052089.8642597</v>
       </c>
       <c r="C24">
-        <v>93.540673889141445</v>
+        <v>5032866733.3700829</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>-35.245692433182334</v>
+        <v>-2165415359.9872589</v>
       </c>
       <c r="B25">
-        <v>-123.27754691136394</v>
+        <v>-7573892728.2954445</v>
       </c>
       <c r="C25">
-        <v>36.163248754376582</v>
+        <v>2221787938.1493745</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <v>-36.037479084957781</v>
+        <v>-2522904928.2109528</v>
       </c>
       <c r="B26">
-        <v>-115.06319342938299</v>
+        <v>-8055321990.5953512</v>
       </c>
       <c r="C26">
-        <v>-16.643700731550826</v>
+        <v>-1165189010.5938303</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <v>-34.760783128203798</v>
+        <v>-2680274829.2768207</v>
       </c>
       <c r="B27">
-        <v>-104.28234938461142</v>
+        <v>-8040824487.8304644</v>
       </c>
       <c r="C27">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <v>-34.760783128203798</v>
+        <v>-2680274829.2768207</v>
       </c>
       <c r="B28">
-        <v>-104.28234938461142</v>
+        <v>-8040824487.8304644</v>
       </c>
       <c r="C28">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <v>-59.602674907367401</v>
+        <v>-4595740801.4254045</v>
       </c>
       <c r="B29">
-        <v>-70.749834298164814</v>
+        <v>-5455256843.4805508</v>
       </c>
       <c r="C29">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <v>-80.69951141879632</v>
+        <v>-6222439477.0680733</v>
       </c>
       <c r="B30">
-        <v>-32.771846923075216</v>
+        <v>-2526915348.6235161</v>
       </c>
       <c r="C30">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <v>-96.725700835740184</v>
+        <v>-7458159395.8349562</v>
       </c>
       <c r="B31">
-        <v>7.2653161206132069</v>
+        <v>560201530.93210602</v>
       </c>
       <c r="C31">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <v>-106.6742587369307</v>
+        <v>-8225255730.569973</v>
       </c>
       <c r="B32">
-        <v>46.845972632479921</v>
+        <v>3612118888.0221529</v>
       </c>
       <c r="C32">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <v>-109.92008064119946</v>
+        <v>-8475528997.3787489</v>
       </c>
       <c r="B33">
-        <v>83.483124396412251</v>
+        <v>6437073530.9337578</v>
       </c>
       <c r="C33">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <v>-106.25921962100338</v>
+        <v>-8193253606.467</v>
       </c>
       <c r="B34">
-        <v>114.87472442506352</v>
+        <v>8857563169.9963627</v>
       </c>
       <c r="C34">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <v>-104.28234938461142</v>
+        <v>-8040824487.8304644</v>
       </c>
       <c r="B35">
-        <v>121.66274094871332</v>
+        <v>9380961902.468874</v>
       </c>
       <c r="C35">
-        <v>-51.413443016777194</v>
+        <v>-3964299558.3870416</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <v>-92.263803582306167</v>
+        <v>-7591876959.1494408</v>
       </c>
       <c r="B36">
-        <v>100.59220149216891</v>
+        <v>8277174657.0934801</v>
       </c>
       <c r="C36">
-        <v>-92.346140495370165</v>
+        <v>-7598652007.3146791</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <v>-73.48486302197395</v>
+        <v>-6464939990.4124413</v>
       </c>
       <c r="B37">
-        <v>74.982104809382804</v>
+        <v>6596662060.8998251</v>
       </c>
       <c r="C37">
-        <v>-124.17185124120164</v>
+        <v>-10924203077.479256</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>-49.590626070832698</v>
+        <v>-4672708927.8122625</v>
       </c>
       <c r="B38">
-        <v>47.413198581285819</v>
+        <v>4467539409.3726921</v>
       </c>
       <c r="C38">
-        <v>-145.18899543354408</v>
+        <v>-13680527328.156466</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>-22.621833462459882</v>
+        <v>-2286589252.8824635</v>
       </c>
       <c r="B39">
-        <v>20.28452021753516</v>
+        <v>2050336282.7006395</v>
       </c>
       <c r="C39">
-        <v>-154.60711353761448</v>
+        <v>-15627511572.877001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <v>5.191038203637329</v>
+        <v>563678789.53045332</v>
       </c>
       <c r="B40">
-        <v>-4.368364897680773</v>
+        <v>-474347238.67504263</v>
       </c>
       <c r="C40">
-        <v>-152.5404704058177</v>
+        <v>-16563898075.824009</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>31.637892791466783</v>
+        <v>3695452596.788269</v>
       </c>
       <c r="B41">
-        <v>-24.997131052005372</v>
+        <v>-2919780829.5028124</v>
       </c>
       <c r="C41">
-        <v>-139.93295681357401</v>
+        <v>-16344818286.142517</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>54.72265049499461</v>
+        <v>6883629675.8720312</v>
       </c>
       <c r="B42">
-        <v>-40.603380219489985</v>
+        <v>-5107549259.6098194</v>
       </c>
       <c r="C42">
-        <v>-118.4260267283086</v>
+        <v>-14896955915.122652</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <v>72.823474961885296</v>
+        <v>9875623846.954565</v>
       </c>
       <c r="B43">
-        <v>-50.743518347792595</v>
+        <v>-6881351104.6557131</v>
       </c>
       <c r="C43">
-        <v>-90.184772745076401</v>
+        <v>-12229997165.33161</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>84.807662541186275</v>
+        <v>12409977476.16609</v>
       </c>
       <c r="B44">
-        <v>-55.484076159828369</v>
+        <v>-8119032110.9836197</v>
       </c>
       <c r="C44">
-        <v>-57.699048390450834</v>
+        <v>-8443150883.612318</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <v>90.094816769996143</v>
+        <v>14237334907.383865</v>
       </c>
       <c r="B45">
-        <v>-55.319087978099084</v>
+        <v>-8741861191.9250717</v>
       </c>
       <c r="C45">
-        <v>-23.576835527937607</v>
+        <v>-3725755992.4284267</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>88.667406521759958</v>
+        <v>15142204569.992846</v>
       </c>
       <c r="B46">
-        <v>-51.062822590561247</v>
+        <v>-8720269780.2802868</v>
       </c>
       <c r="C46">
-        <v>9.6540144891352355</v>
+        <v>1648667397.0810883</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <v>81.032684827953531</v>
+        <v>14963749931.615816</v>
       </c>
       <c r="B47">
-        <v>-43.731297714467942</v>
+        <v>-8075558702.9321804</v>
       </c>
       <c r="C47">
-        <v>39.72172231166261</v>
+        <v>7335137923.5031948</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <v>68.143850456504055</v>
+        <v>13613796322.684772</v>
       </c>
       <c r="B48">
-        <v>-34.424866255988228</v>
+        <v>-6877408812.4624996</v>
       </c>
       <c r="C48">
-        <v>64.753264032825882</v>
+        <v>12936424077.39497</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>51.29104311492955</v>
+        <v>11090335753.865978</v>
       </c>
       <c r="B49">
-        <v>-24.222075475428724</v>
+        <v>-5237385191.7196751</v>
       </c>
       <c r="C49">
-        <v>83.376355983008196</v>
+        <v>18027938712.680698</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
-        <v>31.974200171667572</v>
+        <v>7485057670.444314</v>
       </c>
       <c r="B50">
-        <v>-14.092332668253476</v>
+        <v>-3298969862.1587882</v>
       </c>
       <c r="C50">
-        <v>94.77698135779309</v>
+        <v>22186987242.367931</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
-        <v>11.7700201873662</v>
+        <v>2983820062.5989418</v>
       </c>
       <c r="B51">
-        <v>-4.8320119646902713</v>
+        <v>-1224964274.7798274</v>
       </c>
       <c r="C51">
-        <v>98.712271889850328</v>
+        <v>25024566874.219326</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
-        <v>-7.7955716587256623</v>
+        <v>-2140520146.1181319</v>
       </c>
       <c r="B52">
-        <v>2.9741892741782956</v>
+        <v>816657499.72565889</v>
       </c>
       <c r="C52">
-        <v>95.48177692083992</v>
+        <v>26217534266.066273</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
-        <v>-25.359758316863168</v>
+        <v>-7542910046.9144917</v>
       </c>
       <c r="B53">
-        <v>8.9673485531329558</v>
+        <v>2667214042.4395537</v>
       </c>
       <c r="C53">
-        <v>85.862827805716549</v>
+        <v>25538712885.980648</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
-        <v>-36.540314932992608</v>
+        <v>-11540430498.555363</v>
       </c>
       <c r="B54">
-        <v>12.180104977664206</v>
+        <v>3846810166.1851225</v>
       </c>
       <c r="C54">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <v>-36.540314932992608</v>
+        <v>-11540430498.555363</v>
       </c>
       <c r="B55">
-        <v>12.180104977664206</v>
+        <v>3846810166.1851225</v>
       </c>
       <c r="C55">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
-        <v>-38.421402678985103</v>
+        <v>-12134529439.249212</v>
       </c>
       <c r="B56">
-        <v>20.884651379798761</v>
+        <v>6595943909.5449219</v>
       </c>
       <c r="C56">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
-        <v>-37.888332390622281</v>
+        <v>-11966171267.597511</v>
       </c>
       <c r="B57">
-        <v>28.27693832736562</v>
+        <v>8930630238.8832035</v>
       </c>
       <c r="C57">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
-        <v>-34.974598834617375</v>
+        <v>-11045934546.703182</v>
       </c>
       <c r="B58">
-        <v>33.892481244519516</v>
+        <v>10704172225.751945</v>
       </c>
       <c r="C58">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
-        <v>-29.863282606256583</v>
+        <v>-9431641134.1339302</v>
       </c>
       <c r="B59">
-        <v>37.378434917253486</v>
+        <v>11805131704.485029</v>
       </c>
       <c r="C59">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
-        <v>-22.875546502273963</v>
+        <v>-7224723021.9573565</v>
       </c>
       <c r="B60">
-        <v>38.51576405586885</v>
+        <v>12164331341.987923</v>
       </c>
       <c r="C60">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
-        <v>-14.450455681178445</v>
+        <v>-4563848991.6385765</v>
       </c>
       <c r="B61">
-        <v>37.233006087782435</v>
+        <v>11759201303.99246</v>
       </c>
       <c r="C61">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
-        <v>-12.180104977664213</v>
+        <v>-3846810166.1851244</v>
       </c>
       <c r="B62">
-        <v>36.540314932992608</v>
+        <v>11540430498.555363</v>
       </c>
       <c r="C62">
-        <v>75.143990579429641</v>
+        <v>23732526724.420998</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
-        <v>-18.790541713782311</v>
+        <v>-5478348634.9388094</v>
       </c>
       <c r="B63">
-        <v>52.125426051152552</v>
+        <v>15197074198.424234</v>
       </c>
       <c r="C63">
-        <v>62.083356347816768</v>
+        <v>18100290863.409107</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
-        <v>-25.273283971613882</v>
+        <v>-6802343698.9064322</v>
       </c>
       <c r="B64">
-        <v>65.025078345390753</v>
+        <v>17501600996.944775</v>
       </c>
       <c r="C64">
-        <v>43.262610852263514</v>
+        <v>11644199015.041706</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
-        <v>-30.93796981825577</v>
+        <v>-7688275238.5690241</v>
       </c>
       <c r="B65">
-        <v>74.019414613718681</v>
+        <v>18394278483.400219</v>
       </c>
       <c r="C65">
-        <v>19.619648286144677</v>
+        <v>4875602923.9769783</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
-        <v>-35.026698586788442</v>
+        <v>-8038225943.0717659</v>
       </c>
       <c r="B66">
-        <v>78.099021031775621</v>
+        <v>17922830364.118725</v>
       </c>
       <c r="C66">
-        <v>-7.4627137939678621</v>
+        <v>-1712607297.9946277</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
-        <v>-36.77829084822045</v>
+        <v>-7796369086.7437258</v>
       </c>
       <c r="B67">
-        <v>76.566904434907215</v>
+        <v>16230875145.000256</v>
       </c>
       <c r="C67">
-        <v>-36.223265238271459</v>
+        <v>-7678713143.3064632</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
-        <v>-35.505462926025281</v>
+        <v>-6954829349.4265575</v>
       </c>
       <c r="B68">
-        <v>69.1237380821876</v>
+        <v>13539995334.174063</v>
       </c>
       <c r="C68">
-        <v>-64.624056170816019</v>
+        <v>-12658595199.059866</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
-        <v>-30.679400112751171</v>
+        <v>-5555412988.3646975</v>
       </c>
       <c r="B69">
-        <v>55.927050942689483</v>
+        <v>10127247079.998053</v>
       </c>
       <c r="C69">
-        <v>-90.482686573590925</v>
+        <v>-16384567180.768854</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
-        <v>-22.014368973142275</v>
+        <v>-3687069597.7669988</v>
       </c>
       <c r="B70">
-        <v>37.616263112171865</v>
+        <v>6300147883.94347</v>
       </c>
       <c r="C70">
-        <v>-111.62789148755895</v>
+        <v>-18695961963.240604</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
-        <v>-9.543574100150666</v>
+        <v>-1479317787.8605342</v>
       </c>
       <c r="B71">
-        <v>15.297630025550824</v>
+        <v>2371234924.2983785</v>
       </c>
       <c r="C71">
-        <v>-126.06848249902556</v>
+        <v>-19541457601.974163</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
-        <v>6.3233202054825588</v>
+        <v>907790541.26013398</v>
       </c>
       <c r="B72">
-        <v>-9.5138100356044468</v>
+        <v>-1365824674.5403214</v>
       </c>
       <c r="C72">
-        <v>-132.16360351111859</v>
+        <v>-18973714009.014378</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
-        <v>24.770492809939402</v>
+        <v>3296306549.604497</v>
       </c>
       <c r="B73">
-        <v>-34.994446956347218</v>
+        <v>-4656848193.8198738</v>
       </c>
       <c r="C73">
-        <v>-128.7808829912789</v>
+        <v>-17137376770.221855</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
-        <v>44.582439217748451</v>
+        <v>5504553511.9231358</v>
       </c>
       <c r="B74">
-        <v>-59.149438088063675</v>
+        <v>-7303127708.3267326</v>
       </c>
       <c r="C74">
-        <v>-115.42862073085394</v>
+        <v>-14251867568.688734</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
-        <v>64.192665500236814</v>
+        <v>7361647735.0153408</v>
       </c>
       <c r="B75">
-        <v>-79.977866102396845</v>
+        <v>-9171902619.3404942</v>
       </c>
       <c r="C75">
-        <v>-92.348791802422141</v>
+        <v>-10590606710.375603</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
-        <v>81.77721558373203</v>
+        <v>8721178536.0878239</v>
       </c>
       <c r="B76">
-        <v>-95.652478132724795</v>
+        <v>-10200913949.687931</v>
       </c>
       <c r="C76">
-        <v>-60.559472258402799</v>
+        <v>-6458400006.0018387</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
-        <v>95.391217808557087</v>
+        <v>9472941493.8881779</v>
       </c>
       <c r="B77">
-        <v>-104.69767808256253</v>
+        <v>-10397130907.926037</v>
       </c>
       <c r="C77">
-        <v>-21.838290612855509</v>
+        <v>-2168678145.1651626</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
-        <v>103.14152644964044</v>
+        <v>9551794962.801281</v>
       </c>
       <c r="B78">
-        <v>-106.1476724178566</v>
+        <v>-9830190007.9887505</v>
       </c>
       <c r="C78">
-        <v>21.357416434544287</v>
+        <v>1977880973.2618663</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
-        <v>103.38320469144332</v>
+        <v>8942957160.9071064</v>
       </c>
       <c r="B79">
-        <v>-99.666638444828436</v>
+        <v>-8621463037.8689461</v>
       </c>
       <c r="C79">
-        <v>66.033130862594902</v>
+        <v>5712063794.7648716</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
-        <v>94.922649096237691</v>
+        <v>7683357516.6474485</v>
       </c>
       <c r="B80">
-        <v>-85.614785262563927</v>
+        <v>-6929947806.4118881</v>
       </c>
       <c r="C80">
-        <v>108.85628102946669</v>
+        <v>8811192408.1898632</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
-        <v>82.504743210225129</v>
+        <v>6361634192.9561367</v>
       </c>
       <c r="B81">
-        <v>-70.718351323050101</v>
+        <v>-5452829308.2481165</v>
       </c>
       <c r="C81">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
-        <v>82.504743210225129</v>
+        <v>6361634192.9561367</v>
       </c>
       <c r="B82">
-        <v>-70.718351323050101</v>
+        <v>-5452829308.2481165</v>
       </c>
       <c r="C82">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
-        <v>62.325766175651921</v>
+        <v>4805708251.1600056</v>
       </c>
       <c r="B83">
-        <v>-74.358917211289608</v>
+        <v>-5733539816.9436197</v>
       </c>
       <c r="C83">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
-        <v>38.230632034128583</v>
+        <v>2947821985.7848711</v>
       </c>
       <c r="B84">
-        <v>-73.327238858176017</v>
+        <v>-5653990932.4561319</v>
       </c>
       <c r="C84">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
-        <v>11.733326679471638</v>
+        <v>904713223.71197224</v>
       </c>
       <c r="B85">
-        <v>-67.688140408883044</v>
+        <v>-5219181003.7583351</v>
       </c>
       <c r="C85">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
-        <v>-15.501226742613511</v>
+        <v>-1195241997.5092382</v>
       </c>
       <c r="B86">
-        <v>-57.795947158133139</v>
+        <v>-4456430737.7893677</v>
       </c>
       <c r="C86">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
-        <v>-41.761781078936167</v>
+        <v>-3220095768.2343664</v>
       </c>
       <c r="B87">
-        <v>-44.272221988812781</v>
+        <v>-3413666538.9593115</v>
       </c>
       <c r="C87">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
-        <v>-65.398289120982184</v>
+        <v>-5042619079.1575022</v>
       </c>
       <c r="B88">
-        <v>-27.966710290092418</v>
+        <v>-2156409116.8991194</v>
       </c>
       <c r="C88">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
-        <v>-70.718351323050086</v>
+        <v>-5452829308.2481155</v>
       </c>
       <c r="B89">
-        <v>-23.572783774350043</v>
+        <v>-1817609769.4160395</v>
       </c>
       <c r="C89">
-        <v>137.69255551112178</v>
+        <v>10616961342.732882</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
-        <v>-50.341612770543222</v>
+        <v>-3411775473.1531467</v>
       </c>
       <c r="B90">
-        <v>-15.425834829476068</v>
+        <v>-1045446937.9835505</v>
       </c>
       <c r="C90">
-        <v>174.80639515053576</v>
+        <v>11847061281.951843</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
-        <v>-22.216607833380799</v>
+        <v>-1320667339.7554498</v>
       </c>
       <c r="B91">
-        <v>-6.1983988177388536</v>
+        <v>-368464121.01972061</v>
       </c>
       <c r="C91">
-        <v>203.28545928618257</v>
+        <v>12084314074.40444</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
-        <v>12.761880373708804</v>
+        <v>664020498.96053517</v>
       </c>
       <c r="B92">
-        <v>3.2034169285889358</v>
+        <v>166678768.72458661</v>
       </c>
       <c r="C92">
-        <v>219.70741687881508</v>
+        <v>11431718861.881413</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
-        <v>52.984363776509554</v>
+        <v>2407944989.3662314</v>
       </c>
       <c r="B93">
-        <v>11.784847213441898</v>
+        <v>535578079.55853909</v>
       </c>
       <c r="C93">
-        <v>221.06003004222885</v>
+        <v>10046367527.118011</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
-        <v>96.116658128203909</v>
+        <v>3807196072.581368</v>
       </c>
       <c r="B94">
-        <v>18.56612370681545</v>
+        <v>735407104.61828125</v>
       </c>
       <c r="C94">
-        <v>205.02269820182192</v>
+        <v>8120981592.4193916</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
-        <v>139.14466180021546</v>
+        <v>4793521829.792738</v>
       </c>
       <c r="B95">
-        <v>22.704874973114496</v>
+        <v>782181022.38522673</v>
       </c>
       <c r="C95">
-        <v>170.24201719633939</v>
+        <v>5864823092.8923788</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
-        <v>178.48246140188149</v>
+        <v>5336311637.4098282</v>
       </c>
       <c r="B96">
-        <v>23.628607094150638</v>
+        <v>706453788.35509098</v>
       </c>
       <c r="C96">
-        <v>116.58162638610779</v>
+        <v>3485585556.7318707</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
-        <v>210.14957762521939</v>
+        <v>5441446250.8242826</v>
       </c>
       <c r="B97">
-        <v>21.165347290765872</v>
+        <v>548038692.07924902</v>
       </c>
       <c r="C97">
-        <v>45.325038161742441</v>
+        <v>1173610538.5542455</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
-        <v>230.0192403970743</v>
+        <v>5147369532.6511478</v>
       </c>
       <c r="B98">
-        <v>15.657450048081365</v>
+        <v>350382347.13484597</v>
       </c>
       <c r="C98">
-        <v>-40.690444274768872</v>
+        <v>-910570579.95853078</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
-        <v>234.13437905907338</v>
+        <v>4518935076.1839018</v>
       </c>
       <c r="B99">
-        <v>8.0409786747559338</v>
+        <v>155195750.091162</v>
       </c>
       <c r="C99">
-        <v>-137.03001210983612</v>
+        <v>-2644762083.6443176</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
-        <v>219.08148534289822</v>
+        <v>3639718903.6563859</v>
       </c>
       <c r="B100">
-        <v>-0.12860129118670008</v>
+        <v>-2136522.6268857992</v>
       </c>
       <c r="C100">
-        <v>-237.727144310847</v>
+        <v>-3949489294.8446398</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
-        <v>182.40469529769453</v>
+        <v>2603559351.5944982</v>
       </c>
       <c r="B101">
-        <v>-6.7239377874445569</v>
+        <v>-95974344.725446135</v>
       </c>
       <c r="C101">
-        <v>-335.47466561516512</v>
+        <v>-4788408551.983366</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
-        <v>123.03351775513163</v>
+        <v>1506086042.8900828</v>
       </c>
       <c r="B102">
-        <v>-9.1842707585010928</v>
+        <v>-112427103.2470343</v>
       </c>
       <c r="C102">
-        <v>-421.95154982633687</v>
+        <v>-5165221246.7344446</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
-        <v>41.687992697147322</v>
+        <v>436936318.19115967</v>
       </c>
       <c r="B103">
-        <v>-4.7581472515798451</v>
+        <v>-49870651.163756996</v>
       </c>
       <c r="C103">
-        <v>-488.28880397108168</v>
+        <v>-5117807272.9726038</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
-        <v>-58.784629937028662</v>
+        <v>-526760292.68813974</v>
       </c>
       <c r="B104">
-        <v>9.1442757679822595</v>
+        <v>81940489.973710835</v>
       </c>
       <c r="C104">
-        <v>-525.66864552331344</v>
+        <v>-4710438253.4934931</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
-        <v>-173.19625727367756</v>
+        <v>-1325206940.9149427</v>
       </c>
       <c r="B105">
-        <v>34.496040079212115</v>
+        <v>263945609.83391199</v>
       </c>
       <c r="C105">
-        <v>-526.0400324147131</v>
+        <v>-4024982485.9295421</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
-        <v>-293.98793912268576</v>
+        <v>-1918832510.6413639</v>
       </c>
       <c r="B106">
-        <v>72.118667342508346</v>
+        <v>470711975.23917806</v>
       </c>
       <c r="C106">
-        <v>-482.92047372531232</v>
+        <v>-3151977961.4215913</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
-        <v>-411.44515187474644</v>
+        <v>-2289199011.5479465</v>
       </c>
       <c r="B107">
-        <v>121.1125729108232</v>
+        <v>673846273.14283359</v>
       </c>
       <c r="C107">
-        <v>-392.23915975454196</v>
+        <v>-2182340690.3913174</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
-        <v>-490.55900678017969</v>
+        <v>-2420811666.1558433</v>
       </c>
       <c r="B108">
-        <v>163.51966892672658</v>
+        <v>806937222.05194783</v>
       </c>
       <c r="C108">
-        <v>-292.36996890877174</v>
+        <v>-1442787965.9441867</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">

</xml_diff>